<commit_message>
UFL ESS program info added
</commit_message>
<xml_diff>
--- a/申请截止日期与要求等.xlsx
+++ b/申请截止日期与要求等.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="276">
   <si>
     <t>排名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1000,16 +1000,9 @@
     <t>http://www.che.ufl.edu/Pro_Grad_Std.htm#Admission_Policy</t>
   </si>
   <si>
-    <t>Environmental Engineering Sciences</t>
-  </si>
-  <si>
     <t>http://www.essie.ufl.edu/student_resources/admissions/graduate/</t>
   </si>
   <si>
-    <t>管招生的华裔教授：cywu@essie.ufl.edu     这是一名工作人员： barbi.jackson@essie.ufl.edu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Material Science and Engineering</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1019,6 +1012,18 @@
   </si>
   <si>
     <t>http://www.mse.ufl.edu/admissions/graduate/phd/</t>
+  </si>
+  <si>
+    <t>Environmental Engineering Sciences (EES)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">管招生的华裔教授：cywu@essie.ufl.edu     </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮件中说：不是院系去选学生，而是有招生资格的教授自己选。所以说你如果事先联系好了教授，得到认可，几乎十拿九稳。我是这么理解的，详见附件，邮件全文。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1090,112 +1095,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="86">
     <dxf>
       <fill>
         <patternFill>
@@ -1536,6 +1436,20 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2147,7 +2061,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2381,7 +2295,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="108" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>36</v>
       </c>
@@ -2389,16 +2303,19 @@
         <v>263</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="E11" s="4">
         <v>42353</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="27" x14ac:dyDescent="0.15">
@@ -2409,16 +2326,16 @@
         <v>263</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="E12" s="4">
         <v>42353</v>
       </c>
       <c r="F12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>265</v>
@@ -2437,12 +2354,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H1 A13:H1048576 C5:H5 C6:D6 F6 C7:E7 G7:H7 C8:H10 G11:H11 C11:E12 H12">
-    <cfRule type="expression" dxfId="97" priority="29">
+    <cfRule type="expression" dxfId="85" priority="29">
       <formula>MOD(ROW($A1),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2 F2:H2">
-    <cfRule type="expression" dxfId="96" priority="24">
+    <cfRule type="expression" dxfId="84" priority="24">
       <formula>MOD(ROW($A2),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2452,7 +2369,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="95" priority="21">
+    <cfRule type="expression" dxfId="83" priority="21">
       <formula>MOD(ROW($A2),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2462,7 +2379,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:G3 C4">
-    <cfRule type="expression" dxfId="94" priority="19">
+    <cfRule type="expression" dxfId="82" priority="19">
       <formula>MOD(ROW($A3),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2472,7 +2389,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:B4 G4 D4">
-    <cfRule type="expression" dxfId="93" priority="17">
+    <cfRule type="expression" dxfId="81" priority="17">
       <formula>MOD(ROW($A4),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2482,7 +2399,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:B5">
-    <cfRule type="expression" dxfId="92" priority="15">
+    <cfRule type="expression" dxfId="80" priority="15">
       <formula>MOD(ROW($A5),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2492,7 +2409,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="91" priority="13">
+    <cfRule type="expression" dxfId="79" priority="13">
       <formula>MOD(ROW($A6),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2502,7 +2419,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6">
-    <cfRule type="expression" dxfId="90" priority="11">
+    <cfRule type="expression" dxfId="78" priority="11">
       <formula>MOD(ROW($A6),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2512,7 +2429,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B7">
-    <cfRule type="expression" dxfId="89" priority="9">
+    <cfRule type="expression" dxfId="77" priority="9">
       <formula>MOD(ROW($A7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2522,7 +2439,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:B8">
-    <cfRule type="expression" dxfId="88" priority="7">
+    <cfRule type="expression" dxfId="76" priority="7">
       <formula>MOD(ROW($A8),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2532,7 +2449,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:B10">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="75" priority="5">
       <formula>MOD(ROW($A9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2542,7 +2459,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:B12">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="74" priority="3">
       <formula>MOD(ROW($A11),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2552,7 +2469,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="73" priority="1">
       <formula>MOD(ROW($A12),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2854,7 +2771,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1 F13:G13 A15:G1048576">
-    <cfRule type="expression" dxfId="87" priority="54">
+    <cfRule type="expression" dxfId="72" priority="54">
       <formula>MOD(ROW($A1),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2864,7 +2781,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3 A2:G2">
-    <cfRule type="expression" dxfId="86" priority="47">
+    <cfRule type="expression" dxfId="71" priority="47">
       <formula>MOD(ROW($A2),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2874,7 +2791,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:C3 E3:G3">
-    <cfRule type="expression" dxfId="85" priority="45">
+    <cfRule type="expression" dxfId="70" priority="45">
       <formula>MOD(ROW($A3),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2884,7 +2801,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4 E4:G4">
-    <cfRule type="expression" dxfId="84" priority="43">
+    <cfRule type="expression" dxfId="69" priority="43">
       <formula>MOD(ROW($A4),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2894,7 +2811,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="83" priority="41">
+    <cfRule type="expression" dxfId="68" priority="41">
       <formula>MOD(ROW($A4),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2904,7 +2821,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:C5 E5:G5">
-    <cfRule type="expression" dxfId="82" priority="39">
+    <cfRule type="expression" dxfId="67" priority="39">
       <formula>MOD(ROW($A5),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2914,7 +2831,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="81" priority="37">
+    <cfRule type="expression" dxfId="66" priority="37">
       <formula>MOD(ROW($A5),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2924,7 +2841,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:C6 E6:G6">
-    <cfRule type="expression" dxfId="80" priority="35">
+    <cfRule type="expression" dxfId="65" priority="35">
       <formula>MOD(ROW($A6),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2934,7 +2851,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="79" priority="33">
+    <cfRule type="expression" dxfId="64" priority="33">
       <formula>MOD(ROW($A6),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2944,7 +2861,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C7 E7:G7">
-    <cfRule type="expression" dxfId="78" priority="31">
+    <cfRule type="expression" dxfId="63" priority="31">
       <formula>MOD(ROW($A7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2954,7 +2871,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="77" priority="27">
+    <cfRule type="expression" dxfId="62" priority="27">
       <formula>MOD(ROW($A7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2964,7 +2881,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:C8 F8:G8">
-    <cfRule type="expression" dxfId="76" priority="25">
+    <cfRule type="expression" dxfId="61" priority="25">
       <formula>MOD(ROW($A8),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2974,7 +2891,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="75" priority="23">
+    <cfRule type="expression" dxfId="60" priority="23">
       <formula>MOD(ROW($A8),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2984,7 +2901,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:C9 E9:G9">
-    <cfRule type="expression" dxfId="74" priority="21">
+    <cfRule type="expression" dxfId="59" priority="21">
       <formula>MOD(ROW($A9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2994,7 +2911,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="73" priority="17">
+    <cfRule type="expression" dxfId="58" priority="17">
       <formula>MOD(ROW($A9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3004,7 +2921,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:B10 G10">
-    <cfRule type="expression" dxfId="72" priority="15">
+    <cfRule type="expression" dxfId="57" priority="15">
       <formula>MOD(ROW($A10),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3014,7 +2931,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="71" priority="13">
+    <cfRule type="expression" dxfId="56" priority="13">
       <formula>MOD(ROW($A10),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3024,7 +2941,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="70" priority="11">
+    <cfRule type="expression" dxfId="55" priority="11">
       <formula>MOD(ROW($A10),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3034,7 +2951,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:C11 E11:G11">
-    <cfRule type="expression" dxfId="69" priority="9">
+    <cfRule type="expression" dxfId="54" priority="9">
       <formula>MOD(ROW($A11),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3044,7 +2961,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="68" priority="7">
+    <cfRule type="expression" dxfId="53" priority="7">
       <formula>MOD(ROW($A11),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3054,7 +2971,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:D12 F12:G12">
-    <cfRule type="expression" dxfId="67" priority="5">
+    <cfRule type="expression" dxfId="52" priority="5">
       <formula>MOD(ROW($A12),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3064,7 +2981,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:D13">
-    <cfRule type="expression" dxfId="66" priority="3">
+    <cfRule type="expression" dxfId="51" priority="3">
       <formula>MOD(ROW($A13),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3100,7 +3017,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3855,12 +3772,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:D13 A14 C14:D14 A15:D15 A16:C16 A18:C20 A23:C24 A25:B26 G26 F23:G25 F1:G8 F10:G10 F18:G21 F13:G16 E13:E15 A21:E21 A1:E10 D25:E25 A27:G29 A31:G33 A35:G35 A34:D34 F34:G34 A38:G1048576 F36:G37 A36:D37">
-    <cfRule type="expression" dxfId="64" priority="35">
+    <cfRule type="expression" dxfId="49" priority="35">
       <formula>MOD(ROW($A1),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:E13">
-    <cfRule type="expression" dxfId="63" priority="34">
+    <cfRule type="expression" dxfId="48" priority="34">
       <formula>MOD(ROW($A1)+1,2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3870,7 +3787,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:G9">
-    <cfRule type="expression" dxfId="62" priority="32">
+    <cfRule type="expression" dxfId="47" priority="32">
       <formula>MOD(ROW($A9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3880,7 +3797,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:G11">
-    <cfRule type="expression" dxfId="61" priority="30">
+    <cfRule type="expression" dxfId="46" priority="30">
       <formula>MOD(ROW($A11),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3890,7 +3807,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:G12">
-    <cfRule type="expression" dxfId="60" priority="28">
+    <cfRule type="expression" dxfId="45" priority="28">
       <formula>MOD(ROW($A12),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3900,7 +3817,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="59" priority="26">
+    <cfRule type="expression" dxfId="44" priority="26">
       <formula>MOD(ROW($A14),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3910,7 +3827,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:E16">
-    <cfRule type="expression" dxfId="58" priority="24">
+    <cfRule type="expression" dxfId="43" priority="24">
       <formula>MOD(ROW($A16),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3920,7 +3837,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:C17 F17:G17">
-    <cfRule type="expression" dxfId="57" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>MOD(ROW($A17),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3930,7 +3847,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:E17">
-    <cfRule type="expression" dxfId="56" priority="20">
+    <cfRule type="expression" dxfId="41" priority="20">
       <formula>MOD(ROW($A17),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3940,7 +3857,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:E18">
-    <cfRule type="expression" dxfId="55" priority="18">
+    <cfRule type="expression" dxfId="40" priority="18">
       <formula>MOD(ROW($A18),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3950,7 +3867,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:E19">
-    <cfRule type="expression" dxfId="54" priority="16">
+    <cfRule type="expression" dxfId="39" priority="16">
       <formula>MOD(ROW($A19),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3960,7 +3877,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:E20">
-    <cfRule type="expression" dxfId="53" priority="14">
+    <cfRule type="expression" dxfId="38" priority="14">
       <formula>MOD(ROW($A20),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3970,7 +3887,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22 A22:E22">
-    <cfRule type="expression" dxfId="52" priority="12">
+    <cfRule type="expression" dxfId="37" priority="12">
       <formula>MOD(ROW($A22),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3980,7 +3897,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:E23">
-    <cfRule type="expression" dxfId="51" priority="10">
+    <cfRule type="expression" dxfId="36" priority="10">
       <formula>MOD(ROW($A23),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3990,7 +3907,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:E24">
-    <cfRule type="expression" dxfId="50" priority="8">
+    <cfRule type="expression" dxfId="35" priority="8">
       <formula>MOD(ROW($A24),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4005,7 +3922,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="49" priority="5">
+    <cfRule type="expression" dxfId="34" priority="5">
       <formula>MOD(ROW($A25),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4015,7 +3932,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:F26">
-    <cfRule type="expression" dxfId="48" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>MOD(ROW($A26),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4025,7 +3942,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:G30">
-    <cfRule type="expression" dxfId="47" priority="1">
+    <cfRule type="expression" dxfId="32" priority="1">
       <formula>MOD(ROW($A30),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4551,7 +4468,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F4 A7:F7 C5:F5 C8:F8 A10:C10 G1:G5 G7:G8 E10:G10 A28:G1048576 C22:D22 F22:G22 C23:G23 C24:D25 F24:G25 C26:G26 C27:E27 G27">
-    <cfRule type="expression" dxfId="46" priority="69">
+    <cfRule type="expression" dxfId="31" priority="69">
       <formula>MOD(ROW($A1),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4576,7 +4493,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:B5">
-    <cfRule type="expression" dxfId="45" priority="65">
+    <cfRule type="expression" dxfId="30" priority="65">
       <formula>MOD(ROW($A5),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4586,7 +4503,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:G6">
-    <cfRule type="expression" dxfId="44" priority="63">
+    <cfRule type="expression" dxfId="29" priority="63">
       <formula>MOD(ROW($A6),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4596,7 +4513,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:B8">
-    <cfRule type="expression" dxfId="43" priority="61">
+    <cfRule type="expression" dxfId="28" priority="61">
       <formula>MOD(ROW($A8),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4606,7 +4523,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:C9 E9:G9">
-    <cfRule type="expression" dxfId="42" priority="59">
+    <cfRule type="expression" dxfId="27" priority="59">
       <formula>MOD(ROW($A9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4616,7 +4533,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="41" priority="57">
+    <cfRule type="expression" dxfId="26" priority="57">
       <formula>MOD(ROW($A9),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4626,7 +4543,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="40" priority="53">
+    <cfRule type="expression" dxfId="25" priority="53">
       <formula>MOD(ROW($A10),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4636,7 +4553,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:C11 E11:G11 C12">
-    <cfRule type="expression" dxfId="39" priority="51">
+    <cfRule type="expression" dxfId="24" priority="51">
       <formula>MOD(ROW($A11),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4646,7 +4563,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="38" priority="49">
+    <cfRule type="expression" dxfId="23" priority="49">
       <formula>MOD(ROW($A11),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4656,7 +4573,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:B12 E12:G12">
-    <cfRule type="expression" dxfId="37" priority="47">
+    <cfRule type="expression" dxfId="22" priority="47">
       <formula>MOD(ROW($A12),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4666,7 +4583,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="36" priority="45">
+    <cfRule type="expression" dxfId="21" priority="45">
       <formula>MOD(ROW($A12),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4676,7 +4593,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:C13 E13:G13">
-    <cfRule type="expression" dxfId="35" priority="43">
+    <cfRule type="expression" dxfId="20" priority="43">
       <formula>MOD(ROW($A13),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4686,7 +4603,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="34" priority="41">
+    <cfRule type="expression" dxfId="19" priority="41">
       <formula>MOD(ROW($A13),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4696,7 +4613,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:C14 E14:G14">
-    <cfRule type="expression" dxfId="33" priority="39">
+    <cfRule type="expression" dxfId="18" priority="39">
       <formula>MOD(ROW($A14),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4706,7 +4623,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="32" priority="37">
+    <cfRule type="expression" dxfId="17" priority="37">
       <formula>MOD(ROW($A14),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4716,7 +4633,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:C15 E15:G15">
-    <cfRule type="expression" dxfId="31" priority="35">
+    <cfRule type="expression" dxfId="16" priority="35">
       <formula>MOD(ROW($A15),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4726,7 +4643,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="30" priority="33">
+    <cfRule type="expression" dxfId="15" priority="33">
       <formula>MOD(ROW($A15),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4736,7 +4653,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:C16 E16:G16">
-    <cfRule type="expression" dxfId="29" priority="31">
+    <cfRule type="expression" dxfId="14" priority="31">
       <formula>MOD(ROW($A16),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4746,7 +4663,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="28" priority="27">
+    <cfRule type="expression" dxfId="13" priority="27">
       <formula>MOD(ROW($A16),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4756,7 +4673,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:G17">
-    <cfRule type="expression" dxfId="27" priority="25">
+    <cfRule type="expression" dxfId="12" priority="25">
       <formula>MOD(ROW($A17),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4766,7 +4683,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:D18 G18">
-    <cfRule type="expression" dxfId="26" priority="23">
+    <cfRule type="expression" dxfId="11" priority="23">
       <formula>MOD(ROW($A18),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4776,7 +4693,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="25" priority="21">
+    <cfRule type="expression" dxfId="10" priority="21">
       <formula>MOD(ROW($A18),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4786,7 +4703,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:G19">
-    <cfRule type="expression" dxfId="24" priority="19">
+    <cfRule type="expression" dxfId="9" priority="19">
       <formula>MOD(ROW($A19),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4796,7 +4713,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:G20">
-    <cfRule type="expression" dxfId="23" priority="17">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>MOD(ROW($A20),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4806,7 +4723,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:G21">
-    <cfRule type="expression" dxfId="22" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>MOD(ROW($A21),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4816,7 +4733,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:B22">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="6" priority="13">
       <formula>MOD(ROW($A22),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4826,7 +4743,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:B23">
-    <cfRule type="expression" dxfId="20" priority="11">
+    <cfRule type="expression" dxfId="5" priority="11">
       <formula>MOD(ROW($A23),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4836,7 +4753,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:B24">
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>MOD(ROW($A24),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4846,7 +4763,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:B25">
-    <cfRule type="expression" dxfId="18" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>MOD(ROW($A25),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4856,7 +4773,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B26">
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>MOD(ROW($A26),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4866,7 +4783,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW($A27),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4876,7 +4793,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW($A27),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
UD Dacvis and other 4 emails
</commit_message>
<xml_diff>
--- a/申请截止日期与要求等.xlsx
+++ b/申请截止日期与要求等.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8400" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="其他专业" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="393">
   <si>
     <t>排名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -325,46 +325,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>http://www.chem.upenn.edu/content/graduate-admissions</t>
+  </si>
+  <si>
+    <t>http://www.cbe.seas.upenn.edu/prospective-students/doctoral/index.php</t>
+  </si>
+  <si>
+    <t>成绩要求，gpa至少B，任意一门化学专业课成绩是C的话都不行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Texas A&amp;M University 德州农工大学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.chem.tamu.edu/academics/graduate/admissions/   这里没有什么信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://engineering.tamu.edu/chemical/academics/advising/graduate/admissions</t>
+  </si>
+  <si>
+    <t>GPA要求3.3，往届3.65，往届GRE 164(q),153(v).托福要求80.网页上很详细，提到了同时看重科研经历，可能是如果科研经历很丰富成绩可以稍微放松。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC San Diego  加州大学圣地亚哥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://apply.grad.ucsd.edu/departments/chemical-engineering</t>
+  </si>
+  <si>
     <t>三封推荐信</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://www.chem.upenn.edu/content/graduate-admissions</t>
-  </si>
-  <si>
-    <t>http://www.cbe.seas.upenn.edu/prospective-students/doctoral/index.php</t>
-  </si>
-  <si>
-    <t>成绩要求，gpa至少B，任意一门化学专业课成绩是C的话都不行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Texas A&amp;M University 德州农工大学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.chem.tamu.edu/academics/graduate/admissions/   这里没有什么信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://engineering.tamu.edu/chemical/academics/advising/graduate/admissions</t>
-  </si>
-  <si>
-    <t>GPA要求3.3，往届3.65，往届GRE 164(q),153(v).托福要求80.网页上很详细，提到了同时看重科研经历，可能是如果科研经历很丰富成绩可以稍微放松。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UC San Diego  加州大学圣地亚哥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://apply.grad.ucsd.edu/departments/chemical-engineering</t>
-  </si>
-  <si>
-    <t>三封推荐信</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://apply.grad.ucsd.edu/departments/chemistry-joint-doctoral-program</t>
   </si>
   <si>
@@ -397,10 +393,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>官网三封推荐信。推荐参加biochemistry，chemistry，biology等的sub，详见官网</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Minnesota Twin Cities 明尼苏达双城</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1143,10 +1135,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>gradadm@pitt.edu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://www.chem.pitt.edu/graduate/how-apply</t>
   </si>
   <si>
@@ -1274,10 +1262,6 @@
     <t>http://www.grad-college.iastate.edu/academics/programs/apresults.php?id=27</t>
   </si>
   <si>
-    <t>托福94</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>chemengr@iastate.edu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1356,18 +1340,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>托福要求22，22，23，23。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://chem.virginia.edu/graduate-studies/prospective-graduate-students/application-requirements/     几乎什么信息都没有</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sem8h@virginia.edu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>托福80，GRE verbal 140（硬性要求）.邮件中透露：2015届的gpa平均3.5，GRE总分平均316.GRE q&gt;152被认为是很好的，去年的所有600名申请者都满足这一标准。所以说去年在选择学生的时候他们主要看推荐信和PS。在PS做那个说明你想做哪个方向，为什么，你的研修计划是非常重要的。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1456,6 +1432,49 @@
   </si>
   <si>
     <t>托福80,邮件不提供往届平均分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官网三封推荐信。推荐参加biochemistry，chemistry，biology等的sub，详见官网。邮件：申请者往往具有很深的化学背景，所以化学本科生申请没问题。往届平均gpa 3.7，平均GRE 157</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dsand@ufl.edu</t>
+  </si>
+  <si>
+    <t>托福80，GRE verbal 140（硬性要求）。邮件：你的本科不是化工，所以不能直接申请化工的phD，你需要先读化工的master，完了再去读phD。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三封推荐信，GRE chem sub强烈推荐。去年平均gpa 3.7，平均GRE q 163，平均chem sub 761.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gradadm@pitt.edu   老师回复地很热情，不知道是因为看中了你的北大背景还是仅仅是性格热情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>agl2107@columbia.edu           中国学长 jw3227@columbia.edu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>托福要求22，22，23，23。邮件：平均gpa 3.5，他说没有平均GRE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sem8h@virginia.edu       这里是所有在读学生： http://chem.virginia.edu/graduate-studies/current-graduate-students/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目全称  Chemical and Biological Engineering</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>托福94，邮件：录取学生的GRE范围 v:150-164,q 160-170, w: 3-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮件：录取者都有strong recommendation letters和科研经历。2015届平均gpa 3.6，平均GRE v:161, q:161, w:4.5，更多年份详见附件截图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2677,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2743,19 +2762,19 @@
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="E3" s="4">
         <v>42353</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="54" x14ac:dyDescent="0.15">
@@ -2763,23 +2782,23 @@
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
@@ -2787,25 +2806,25 @@
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E5" s="4">
         <v>42339</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="54" x14ac:dyDescent="0.15">
@@ -2813,19 +2832,19 @@
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E6" s="4">
         <v>42353</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="121.5" x14ac:dyDescent="0.15">
@@ -2833,25 +2852,25 @@
         <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="E7" s="4">
         <v>42036</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
@@ -2859,22 +2878,22 @@
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E8" s="4">
         <v>42019</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
@@ -2882,22 +2901,22 @@
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E9" s="4">
         <v>42353</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
@@ -2905,22 +2924,22 @@
         <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E10" s="4">
         <v>42352</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="108" x14ac:dyDescent="0.15">
@@ -2928,22 +2947,22 @@
         <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E11" s="4">
         <v>42353</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="27" x14ac:dyDescent="0.15">
@@ -2951,22 +2970,22 @@
         <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="E12" s="4">
         <v>42353</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
@@ -2974,19 +2993,19 @@
         <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E13" s="4">
         <v>42019</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="27" x14ac:dyDescent="0.15">
@@ -2994,22 +3013,22 @@
         <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E14" s="4">
         <v>42035</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="94.5" x14ac:dyDescent="0.15">
@@ -3017,25 +3036,25 @@
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E15" s="4">
         <v>42019</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="81" x14ac:dyDescent="0.15">
@@ -3043,22 +3062,22 @@
         <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E16" s="4">
         <v>42346</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3066,19 +3085,19 @@
         <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E17" s="4">
         <v>42019</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3283,8 +3302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3305,10 +3324,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>16</v>
@@ -3328,7 +3347,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D2" s="4">
         <v>42339</v>
@@ -3346,16 +3365,16 @@
         <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D3" s="4">
         <v>42339</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
@@ -3366,13 +3385,13 @@
         <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D4" s="4">
         <v>42353</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>72</v>
@@ -3389,7 +3408,7 @@
         <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D5" s="4">
         <v>42339</v>
@@ -3409,7 +3428,7 @@
         <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D6" s="4">
         <v>42115</v>
@@ -3426,33 +3445,33 @@
         <v>73</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D8" s="4">
         <v>42019</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>103</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="67.5" x14ac:dyDescent="0.15">
@@ -3460,22 +3479,22 @@
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D9" s="4">
         <v>42339</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.15">
@@ -3483,19 +3502,19 @@
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D10" s="4">
         <v>42339</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -3503,19 +3522,19 @@
         <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D11" s="4">
         <v>42339</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="2" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
@@ -3523,17 +3542,17 @@
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -3541,19 +3560,19 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D13" s="4">
         <v>42339</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G13" s="2"/>
     </row>
@@ -3562,19 +3581,19 @@
         <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D14" s="4">
         <v>42339</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -3583,30 +3602,33 @@
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E15" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="108" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D16" s="4">
         <v>42339</v>
       </c>
       <c r="E16" t="s">
-        <v>297</v>
+        <v>295</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>392</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -3614,13 +3636,13 @@
         <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E17" t="s">
         <v>319</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E17" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -3628,16 +3650,16 @@
         <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D18" s="4">
         <v>42005</v>
       </c>
       <c r="F18" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="81" x14ac:dyDescent="0.15">
@@ -3645,19 +3667,19 @@
         <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D19" s="4">
         <v>42019</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="81" x14ac:dyDescent="0.15">
@@ -3665,19 +3687,19 @@
         <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D20" s="4">
         <v>42339</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -3685,19 +3707,19 @@
         <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D21" s="4">
         <v>42353</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F21" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -4039,8 +4061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4067,7 +4089,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
@@ -4166,7 +4188,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -4202,7 +4224,7 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="121.5" x14ac:dyDescent="0.15">
@@ -4238,7 +4260,7 @@
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="121.5" x14ac:dyDescent="0.15">
@@ -4254,7 +4276,9 @@
       <c r="D11" s="4">
         <v>42353</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>387</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>58</v>
       </c>
@@ -4309,7 +4333,7 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -4347,10 +4371,10 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4385,13 +4409,13 @@
         <v>42339</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -4399,14 +4423,14 @@
         <v>82</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="4">
         <v>42353</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="2" t="s">
-        <v>83</v>
+        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -4414,19 +4438,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="D20" s="4">
         <v>42353</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4434,16 +4458,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -4451,22 +4475,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="4">
         <v>42019</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="G22" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -4474,10 +4498,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D23" s="4">
         <v>42019</v>
@@ -4489,19 +4513,19 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D24" s="4">
         <v>42009</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="54" x14ac:dyDescent="0.15">
@@ -4509,19 +4533,19 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D25" s="4">
         <v>42349</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="54" x14ac:dyDescent="0.15">
@@ -4529,17 +4553,17 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D26" s="4">
         <v>42005</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
@@ -4547,19 +4571,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4567,19 +4591,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D28" s="4">
         <v>42353</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="162" x14ac:dyDescent="0.15">
@@ -4587,22 +4611,22 @@
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D29" s="4">
         <v>42019</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4610,19 +4634,19 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D30" s="4">
         <v>42353</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4630,19 +4654,19 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D31" s="4">
         <v>42353</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4650,22 +4674,22 @@
         <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D32" s="4">
         <v>42353</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="121.5" x14ac:dyDescent="0.15">
@@ -4673,19 +4697,19 @@
         <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D33" s="4">
         <v>42339</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -4693,19 +4717,19 @@
         <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D34" s="4">
         <v>42339</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4713,13 +4737,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4727,16 +4751,16 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D36" s="4">
         <v>42358</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4744,19 +4768,19 @@
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D37" s="4">
         <v>42353</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="175.5" x14ac:dyDescent="0.15">
@@ -4764,22 +4788,22 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D38" s="4">
         <v>42008</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="54" x14ac:dyDescent="0.15">
@@ -4787,19 +4811,19 @@
         <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="D39" s="4">
         <v>42353</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -4807,19 +4831,19 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D40" s="4">
         <v>42353</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -4827,36 +4851,36 @@
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D41" s="4">
         <v>42339</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>303</v>
+        <v>386</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="162" x14ac:dyDescent="0.15">
@@ -4864,22 +4888,22 @@
         <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D43" s="4">
         <v>42007</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="108" x14ac:dyDescent="0.15">
@@ -4887,19 +4911,19 @@
         <v>38</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D44" s="4">
         <v>42339</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4907,16 +4931,16 @@
         <v>38</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D45" s="4">
         <v>42005</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="27" x14ac:dyDescent="0.15">
@@ -4924,19 +4948,19 @@
         <v>38</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D46" s="4">
         <v>42019</v>
       </c>
       <c r="E46" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="121.5" x14ac:dyDescent="0.15">
@@ -4944,39 +4968,39 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D47" s="4">
         <v>42339</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="135" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D48" s="4">
         <v>42019</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>362</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="27" x14ac:dyDescent="0.15">
@@ -4984,16 +5008,16 @@
         <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D49" s="4">
         <v>42006</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -5212,8 +5236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5301,7 +5325,7 @@
         <v>42369</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="121.5" x14ac:dyDescent="0.15">
@@ -5397,7 +5421,7 @@
         <v>42353</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="54" x14ac:dyDescent="0.15">
@@ -5425,11 +5449,11 @@
         <v>82</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="4"/>
       <c r="F12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="108" x14ac:dyDescent="0.15">
@@ -5437,16 +5461,16 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="4">
         <v>42353</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
@@ -5454,16 +5478,16 @@
         <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D14" s="4">
         <v>42353</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="54" x14ac:dyDescent="0.15">
@@ -5471,19 +5495,19 @@
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="4">
         <v>42009</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -5491,19 +5515,19 @@
         <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D16" s="4">
         <v>42005</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="81" x14ac:dyDescent="0.15">
@@ -5511,19 +5535,19 @@
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D17" s="4">
         <v>42012</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="54" x14ac:dyDescent="0.15">
@@ -5531,19 +5555,19 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D18" s="4">
         <v>42353</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="202.5" x14ac:dyDescent="0.15">
@@ -5551,19 +5575,19 @@
         <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D19" s="4">
         <v>42005</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -5571,22 +5595,22 @@
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D20" s="4">
         <v>42036</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="108" x14ac:dyDescent="0.15">
@@ -5594,19 +5618,19 @@
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D21" s="4">
         <v>42338</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="81" x14ac:dyDescent="0.15">
@@ -5614,19 +5638,19 @@
         <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
@@ -5634,19 +5658,19 @@
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D23" s="4">
         <v>42353</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="54" x14ac:dyDescent="0.15">
@@ -5654,16 +5678,16 @@
         <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" t="s">
         <v>217</v>
       </c>
-      <c r="C24" t="s">
-        <v>219</v>
-      </c>
       <c r="E24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="148.5" x14ac:dyDescent="0.15">
@@ -5671,22 +5695,22 @@
         <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D25" s="4">
         <v>42014</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -5694,36 +5718,39 @@
         <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D26" s="4">
         <v>42358</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D27" s="4">
         <v>42019</v>
       </c>
+      <c r="E27" t="s">
+        <v>383</v>
+      </c>
       <c r="F27" s="2" t="s">
-        <v>246</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="121.5" x14ac:dyDescent="0.15">
@@ -5731,22 +5758,22 @@
         <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D28" s="4">
         <v>42353</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -5754,19 +5781,19 @@
         <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D29" s="4">
         <v>42036</v>
       </c>
       <c r="E29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
@@ -5774,16 +5801,16 @@
         <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D30" s="4">
         <v>42019</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="175.5" x14ac:dyDescent="0.15">
@@ -5791,22 +5818,22 @@
         <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D31" s="4">
         <v>42064</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -5814,69 +5841,72 @@
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D32" s="4">
         <v>42353</v>
       </c>
       <c r="E32" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="D33" s="4">
         <v>42035</v>
       </c>
       <c r="E33" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D34" s="4">
         <v>42005</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>339</v>
+        <v>391</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:F4 A7:F7 C5:F5 C8:F8 A10:C10 G1:G5 A36:G1048576 G7:G8 E10:G10 C22:D22 F22:G22 C23:G23 C24:D25 F24:G25 C26:G26 C27:E27 G27 C28 F28:G29 C29:D29 C30:G35">
+  <conditionalFormatting sqref="A1:F4 A7:F7 C5:F5 C8:F8 A10:C10 G1:G5 A36:G1048576 G7:G8 E10:G10 C22:D22 F22:G22 C23:G23 C24:D25 F24:G25 C26:G26 C27:D27 G27 C28 F28:G29 C29:D29 C30:G35">
     <cfRule type="expression" priority="88" stopIfTrue="1">
       <formula>MOD(ROW+$A$1:$F$1,2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F4 A7:F7 C5:F5 C8:F8 A10:C10 G1:G5 G7:G8 E10:G10 A36:G1048576 C22:D22 F22:G22 C23:G23 C24:D25 F24:G25 C26:G26 C27:E27 G27 C28 F28:G29 C29:D29 C30:G35">
+  <conditionalFormatting sqref="A1:F4 A7:F7 C5:F5 C8:F8 A10:C10 G1:G5 G7:G8 E10:G10 A36:G1048576 C22:D22 F22:G22 C23:G23 C24:D25 F24:G25 C26:G26 C27:D27 G27 C28 F28:G29 C29:D29 C30:G35">
     <cfRule type="expression" dxfId="40" priority="87">
       <formula>MOD(ROW($A1),2)</formula>
     </cfRule>

</xml_diff>